<commit_message>
se actualizo clase equivalencia a Registrar rol
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M4.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b6b49da01230f2/Documentos/proyecto wong/Softgenix-Peru/2-Desarrollo/SCIP/pruebas-calidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="11_8BF91C39AE0E0FE7D079E26E9C7D4D10BFF76F8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91288332-2B4A-44A1-A4C1-E1CB75416D5F}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_8BF91C39AE0E0FE7D079E26E9C7D4D10BFF76F8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB55BCD9-D43B-4B6D-BF6E-DBB02D74EAC8}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="2640" windowWidth="17925" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CE Registrar rol" sheetId="1" r:id="rId1"/>
@@ -476,46 +476,46 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,6 +531,115 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>585082</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>47227</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7FD3C19-0BD9-D9EC-A902-5CC50C1098F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="361950" y="2705100"/>
+          <a:ext cx="6566782" cy="3942952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>646100</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>118921</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94751075-B8A3-EAC6-5859-B1E7E421947B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7096125" y="857250"/>
+          <a:ext cx="7227875" cy="3919396"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -734,7 +843,7 @@
   <dimension ref="B1:P985"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -752,62 +861,62 @@
     <row r="2" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="40" t="s">
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="40" t="s">
+      <c r="E4" s="40"/>
+      <c r="F4" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="41"/>
+      <c r="G4" s="40"/>
     </row>
     <row r="5" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="42" t="s">
+      <c r="E5" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="42" t="s">
+      <c r="F5" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="42" t="s">
+      <c r="G5" s="33" t="s">
         <v>5</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="34"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="37"/>
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="2:16" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="E6" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="45" t="s">
+      <c r="F6" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="45" t="s">
+      <c r="G6" s="35" t="s">
         <v>35</v>
       </c>
       <c r="I6" s="2"/>
@@ -820,20 +929,20 @@
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="41"/>
-      <c r="C7" s="43" t="s">
+      <c r="B7" s="40"/>
+      <c r="C7" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="47" t="s">
+      <c r="E7" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="45" t="s">
+      <c r="F7" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="45" t="s">
+      <c r="G7" s="35" t="s">
         <v>40</v>
       </c>
       <c r="I7" s="2"/>
@@ -842,18 +951,18 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="35"/>
+      <c r="O7" s="36"/>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="2:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="45" t="s">
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="45" t="s">
+      <c r="G8" s="35" t="s">
         <v>42</v>
       </c>
       <c r="I8" s="2"/>
@@ -862,7 +971,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="34"/>
+      <c r="O8" s="37"/>
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -872,7 +981,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="35"/>
+      <c r="O9" s="36"/>
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -882,7 +991,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-      <c r="O10" s="34"/>
+      <c r="O10" s="37"/>
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -892,7 +1001,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="35"/>
+      <c r="O11" s="36"/>
       <c r="P11" s="1"/>
     </row>
     <row r="12" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -902,7 +1011,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
-      <c r="O12" s="34"/>
+      <c r="O12" s="37"/>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1961,20 +2070,21 @@
     <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="D4:E4"/>
     <mergeCell ref="O7:O8"/>
     <mergeCell ref="O9:O10"/>
     <mergeCell ref="O11:O12"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="N5:O5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1998,20 +2108,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="32"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="47"/>
     </row>
     <row r="3" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -2041,11 +2151,11 @@
       <c r="I3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="37" t="s">
+      <c r="J3" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="32"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="47"/>
     </row>
     <row r="4" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">

</xml_diff>

<commit_message>
Se agrego  casos de prueba correctos a Registrar rol
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M4.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M4.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b6b49da01230f2/Documentos/proyecto wong/Softgenix-Peru/2-Desarrollo/SCIP/pruebas-calidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_8BF91C39AE0E0FE7D079E26E9C7D4D10BFF76F8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB55BCD9-D43B-4B6D-BF6E-DBB02D74EAC8}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="11_8BF91C39AE0E0FE7D079E26E9C7D4D10BFF76F8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A82628C-DA74-4E28-B108-A61BB5A004C0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1875" yWindow="1545" windowWidth="17925" windowHeight="11460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CE Registrar rol" sheetId="1" r:id="rId1"/>
-    <sheet name="2.0CP Generar reporte de Invent" sheetId="2" r:id="rId2"/>
+    <sheet name="CP Registrar rol" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -46,12 +46,6 @@
     <t>Código</t>
   </si>
   <si>
-    <t>AGREGAR USUARIO</t>
-  </si>
-  <si>
-    <t>CONDICIONES DE ENTRADA</t>
-  </si>
-  <si>
     <t>Caso prueba</t>
   </si>
   <si>
@@ -61,21 +55,6 @@
     <t>Clases de equivalencia</t>
   </si>
   <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Usuario</t>
-  </si>
-  <si>
-    <t>Contraseña</t>
-  </si>
-  <si>
-    <t>Tipo de Perfil</t>
-  </si>
-  <si>
-    <t>Foto</t>
-  </si>
-  <si>
     <t>Resultado esperado</t>
   </si>
   <si>
@@ -88,36 +67,6 @@
     <t>CP02</t>
   </si>
   <si>
-    <t>CP03</t>
-  </si>
-  <si>
-    <t>CP04</t>
-  </si>
-  <si>
-    <t>CP05</t>
-  </si>
-  <si>
-    <t>CP06</t>
-  </si>
-  <si>
-    <t>CP07</t>
-  </si>
-  <si>
-    <t>CP08</t>
-  </si>
-  <si>
-    <t>CP09</t>
-  </si>
-  <si>
-    <t>CP10</t>
-  </si>
-  <si>
-    <t>CP11</t>
-  </si>
-  <si>
-    <t>CP12</t>
-  </si>
-  <si>
     <t>Descripcion</t>
   </si>
   <si>
@@ -155,13 +104,37 @@
   </si>
   <si>
     <t>CENV&lt;03&gt;</t>
+  </si>
+  <si>
+    <t>REGISTRAR ROL</t>
+  </si>
+  <si>
+    <t>CONDICIONES DE  ENTRADA</t>
+  </si>
+  <si>
+    <t>Registro exitoso</t>
+  </si>
+  <si>
+    <t>CEV&lt;01&gt;,CEV&lt;02&gt;</t>
+  </si>
+  <si>
+    <t>adminisrador</t>
+  </si>
+  <si>
+    <t>Modificado correctamente</t>
+  </si>
+  <si>
+    <t>Modificado Correctamente</t>
+  </si>
+  <si>
+    <t>ADMINISTRADOR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -182,11 +155,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -196,31 +164,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -248,7 +191,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -273,95 +216,13 @@
         <bgColor rgb="FFDAEEF3"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB6D7A8"/>
-        <bgColor rgb="FFB6D7A8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB4A7D6"/>
-        <bgColor rgb="FFB4A7D6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE6B8AF"/>
-        <bgColor rgb="FFE6B8AF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF9CB9C"/>
-        <bgColor rgb="FFF9CB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9FC5E8"/>
-        <bgColor rgb="FF9FC5E8"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -383,139 +244,70 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -842,7 +634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P985"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
@@ -861,63 +653,63 @@
     <row r="2" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="43" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="40"/>
-      <c r="F4" s="43" t="s">
+      <c r="E4" s="10"/>
+      <c r="F4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="40"/>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="33" t="s">
+      <c r="F5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="33" t="s">
+      <c r="G5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="38"/>
-      <c r="O5" s="37"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="15"/>
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="2:16" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="35" t="s">
-        <v>35</v>
+      <c r="B6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -929,21 +721,21 @@
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="40"/>
-      <c r="C7" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="35" t="s">
-        <v>40</v>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -951,19 +743,19 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="36"/>
+      <c r="O7" s="14"/>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="2:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="35" t="s">
-        <v>42</v>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -971,7 +763,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="37"/>
+      <c r="O8" s="15"/>
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -981,7 +773,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="36"/>
+      <c r="O9" s="14"/>
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -991,7 +783,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-      <c r="O10" s="37"/>
+      <c r="O10" s="15"/>
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1001,7 +793,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="36"/>
+      <c r="O11" s="14"/>
       <c r="P11" s="1"/>
     </row>
     <row r="12" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1011,7 +803,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
-      <c r="O12" s="37"/>
+      <c r="O12" s="15"/>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2070,17 +1862,17 @@
     <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="D4:E4"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -2090,263 +1882,130 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L991"/>
+  <dimension ref="A1:K977"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="8" width="12" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.42578125" customWidth="1"/>
     <col min="10" max="28" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+    </row>
+    <row r="2" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+    </row>
+    <row r="5" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
+      <c r="C5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
     </row>
-    <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="47"/>
+    <row r="6" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
     </row>
-    <row r="3" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="6" t="s">
+    <row r="7" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="46"/>
-      <c r="L3" s="47"/>
+      <c r="C7" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
     </row>
-    <row r="4" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-    </row>
-    <row r="5" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-    </row>
-    <row r="6" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-    </row>
-    <row r="7" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-    </row>
-    <row r="8" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-    </row>
-    <row r="9" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-    </row>
-    <row r="10" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-    </row>
-    <row r="11" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-    </row>
-    <row r="12" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-    </row>
-    <row r="13" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-    </row>
-    <row r="14" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-    </row>
-    <row r="15" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="29"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="29"/>
-    </row>
-    <row r="16" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3308,25 +2967,16 @@
     <row r="975" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="976" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="977" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="978" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="979" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="980" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="981" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="982" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="983" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="984" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="986" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="987" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="988" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="989" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="8">
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="I7:K7"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Se agrego  casos de prueba con datos incorrectos a Registrar rol
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M4.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b6b49da01230f2/Documentos/proyecto wong/Softgenix-Peru/2-Desarrollo/SCIP/pruebas-calidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_8BF91C39AE0E0FE7D079E26E9C7D4D10BFF76F8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A82628C-DA74-4E28-B108-A61BB5A004C0}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="11_8BF91C39AE0E0FE7D079E26E9C7D4D10BFF76F8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81E21D29-A652-4EAB-9258-981F58438CAD}"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="1545" windowWidth="17925" windowHeight="11460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="2310" windowWidth="17925" windowHeight="11460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CE Registrar rol" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -128,13 +128,40 @@
   </si>
   <si>
     <t>ADMINISTRADOR</t>
+  </si>
+  <si>
+    <t>CP03</t>
+  </si>
+  <si>
+    <t>Registro  con descripcion incorrecta</t>
+  </si>
+  <si>
+    <t>CEV&lt;02&gt;,CENV&lt;01&gt;</t>
+  </si>
+  <si>
+    <t>registro fallido</t>
+  </si>
+  <si>
+    <t>CP04</t>
+  </si>
+  <si>
+    <t>4dmin1strad0r</t>
+  </si>
+  <si>
+    <t>CP05</t>
+  </si>
+  <si>
+    <t>CEV&lt;02&gt;,CENV&lt;02&gt;</t>
+  </si>
+  <si>
+    <t>Administ@dor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -190,8 +217,16 @@
       <name val="Garamond"/>
       <family val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,6 +249,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDAEEF3"/>
         <bgColor rgb="FFDAEEF3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6D7A8"/>
+        <bgColor rgb="FFB6D7A8"/>
       </patternFill>
     </fill>
   </fills>
@@ -241,10 +282,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -268,6 +310,23 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -283,33 +342,29 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -655,14 +710,14 @@
     <row r="4" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="9" t="s">
+      <c r="E4" s="17"/>
+      <c r="F4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="17"/>
     </row>
     <row r="5" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
@@ -686,14 +741,14 @@
       <c r="I5" s="1"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="14"/>
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="2:16" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="18" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -721,14 +776,14 @@
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="10"/>
-      <c r="C7" s="11" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="20" t="s">
         <v>21</v>
       </c>
       <c r="F7" s="8" t="s">
@@ -743,14 +798,14 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="14"/>
+      <c r="O7" s="13"/>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="2:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
       <c r="F8" s="8" t="s">
         <v>24</v>
       </c>
@@ -763,7 +818,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="15"/>
+      <c r="O8" s="14"/>
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -773,7 +828,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="14"/>
+      <c r="O9" s="13"/>
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -783,7 +838,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-      <c r="O10" s="15"/>
+      <c r="O10" s="14"/>
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -793,7 +848,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="14"/>
+      <c r="O11" s="13"/>
       <c r="P11" s="1"/>
     </row>
     <row r="12" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -803,7 +858,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
-      <c r="O12" s="15"/>
+      <c r="O12" s="14"/>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1862,17 +1917,17 @@
     <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="D4:E4"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -1884,48 +1939,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K977"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.42578125" customWidth="1"/>
-    <col min="10" max="28" width="10" customWidth="1"/>
+    <col min="8" max="9" width="25.42578125" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="11" max="11" width="4.5703125" customWidth="1"/>
+    <col min="12" max="28" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="9" t="s">
+    <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
     </row>
-    <row r="5" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
@@ -1935,71 +1991,138 @@
       <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
       <c r="H5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
     </row>
-    <row r="6" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="21" t="s">
+    <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="22" t="s">
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="24" t="s">
+      <c r="I6" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
     </row>
-    <row r="7" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="21" t="s">
+    <row r="7" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="22" t="s">
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="24" t="s">
+      <c r="I7" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
     </row>
-    <row r="8" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+    </row>
+    <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+    </row>
+    <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+    </row>
     <row r="11" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2968,16 +3091,25 @@
     <row r="976" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="977" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="14">
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="I8:K8"/>
     <mergeCell ref="I5:K5"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="I7:K7"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E10" r:id="rId1" xr:uid="{A5164392-496C-4A39-9165-C13CA7099E7B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>

<commit_message>
Se actualizo  casos de prueba a Registrar rol
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M4.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b6b49da01230f2/Documentos/proyecto wong/Softgenix-Peru/2-Desarrollo/SCIP/pruebas-calidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="11_8BF91C39AE0E0FE7D079E26E9C7D4D10BFF76F8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81E21D29-A652-4EAB-9258-981F58438CAD}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="11_8BF91C39AE0E0FE7D079E26E9C7D4D10BFF76F8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{792DB987-D3D7-4F1B-B249-1AACCC319791}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2310" windowWidth="17925" windowHeight="11460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7320" yWindow="3630" windowWidth="17925" windowHeight="11460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CE Registrar rol" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -155,6 +155,21 @@
   </si>
   <si>
     <t>Administ@dor</t>
+  </si>
+  <si>
+    <t>CP06</t>
+  </si>
+  <si>
+    <t>Registro con descripcion incorrecta</t>
+  </si>
+  <si>
+    <t>CEV&lt;01&gt;,CENV&lt;03&gt;</t>
+  </si>
+  <si>
+    <t>ASDFFDSDSFDFDGDSDFSDSDFSDFSDFDSFFFSDDFFFDSSDFDSGSDESDFSDFFSDFSDFSD</t>
+  </si>
+  <si>
+    <t>ERROR</t>
   </si>
 </sst>
 </file>
@@ -226,7 +241,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -255,6 +270,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB6D7A8"/>
         <bgColor rgb="FFB6D7A8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB1A0C7"/>
+        <bgColor rgb="FFB4A7D6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB1A0C7"/>
+        <bgColor rgb="FFB6D7A8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4A7D6"/>
+        <bgColor rgb="FFB4A7D6"/>
       </patternFill>
     </fill>
   </fills>
@@ -286,7 +319,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -320,12 +353,14 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -342,24 +377,31 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -741,10 +783,10 @@
       <c r="I5" s="1"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="14"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="22"/>
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="2:16" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -798,7 +840,7 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="13"/>
+      <c r="O7" s="21"/>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="2:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -818,7 +860,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="14"/>
+      <c r="O8" s="22"/>
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -828,7 +870,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="13"/>
+      <c r="O9" s="21"/>
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -838,7 +880,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-      <c r="O10" s="14"/>
+      <c r="O10" s="22"/>
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -848,7 +890,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="13"/>
+      <c r="O11" s="21"/>
       <c r="P11" s="1"/>
     </row>
     <row r="12" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -858,7 +900,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
-      <c r="O12" s="14"/>
+      <c r="O12" s="22"/>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1917,17 +1959,17 @@
     <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="D4:E4"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -1939,8 +1981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K977"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1959,11 +2001,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
     </row>
     <row r="2" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1991,19 +2033,19 @@
       <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
       <c r="H5" s="6" t="s">
         <v>9</v>
       </c>
       <c r="I5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="10" t="s">
@@ -2015,19 +2057,19 @@
       <c r="D6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
       <c r="H6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="23" t="s">
+      <c r="I6" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
     </row>
     <row r="7" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="10" t="s">
@@ -2039,91 +2081,114 @@
       <c r="D7" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
       <c r="H7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="23" t="s">
+      <c r="I7" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
     </row>
     <row r="8" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="14" t="s">
         <v>35</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="27" t="s">
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
     </row>
     <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="14" t="s">
         <v>35</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="27" t="s">
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="23" t="s">
+      <c r="I9" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
     </row>
     <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="14" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="27" t="s">
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="23" t="s">
+      <c r="I10" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
     </row>
-    <row r="11" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+    </row>
     <row r="12" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3091,7 +3156,9 @@
     <row r="976" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="977" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="16">
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="I11:K11"/>
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="E10:G10"/>

</xml_diff>

<commit_message>
Se agrego  clase equivalencia a Borrar rol
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M4.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M4.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b6b49da01230f2/Documentos/proyecto wong/Softgenix-Peru/2-Desarrollo/SCIP/pruebas-calidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="11_8BF91C39AE0E0FE7D079E26E9C7D4D10BFF76F8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{792DB987-D3D7-4F1B-B249-1AACCC319791}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="11_8BF91C39AE0E0FE7D079E26E9C7D4D10BFF76F8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31F28D13-2AE5-4571-B8B5-43F18455D871}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="3630" windowWidth="17925" windowHeight="11460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="960" windowWidth="17925" windowHeight="11460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CE Registrar rol" sheetId="1" r:id="rId1"/>
     <sheet name="CP Registrar rol" sheetId="2" r:id="rId2"/>
+    <sheet name="CE Borrar rol" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -170,6 +171,27 @@
   </si>
   <si>
     <t>ERROR</t>
+  </si>
+  <si>
+    <t>Borrar</t>
+  </si>
+  <si>
+    <t>Hacer clic en el botón de borrar</t>
+  </si>
+  <si>
+    <t>No hacer clic en el botón de borrar</t>
+  </si>
+  <si>
+    <t>logico</t>
+  </si>
+  <si>
+    <t>Confirmar la acción de borrado cuando se solicite</t>
+  </si>
+  <si>
+    <t>Hacer clic en un área no interactiva</t>
+  </si>
+  <si>
+    <t>Cancelar la acción de borrado cuando se solicite</t>
   </si>
 </sst>
 </file>
@@ -362,6 +384,22 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -377,13 +415,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -395,15 +426,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -516,6 +538,61 @@
         <a:xfrm>
           <a:off x="7096125" y="857250"/>
           <a:ext cx="7227875" cy="3919396"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>648286</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>123978</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C6C90BD-D1D2-C12C-F47D-0F6E307217F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3667125" y="3733800"/>
+          <a:ext cx="4201111" cy="1095528"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -752,14 +829,14 @@
     <row r="4" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="16" t="s">
+      <c r="E4" s="23"/>
+      <c r="F4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="17"/>
+      <c r="G4" s="23"/>
     </row>
     <row r="5" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
@@ -783,14 +860,14 @@
       <c r="I5" s="1"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="22"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="20"/>
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="2:16" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="24" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -818,14 +895,14 @@
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="17"/>
-      <c r="C7" s="18" t="s">
+      <c r="B7" s="23"/>
+      <c r="C7" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="26" t="s">
         <v>21</v>
       </c>
       <c r="F7" s="8" t="s">
@@ -840,14 +917,14 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="21"/>
+      <c r="O7" s="19"/>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="2:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
       <c r="F8" s="8" t="s">
         <v>24</v>
       </c>
@@ -860,7 +937,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="22"/>
+      <c r="O8" s="20"/>
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -870,7 +947,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="21"/>
+      <c r="O9" s="19"/>
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -880,7 +957,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-      <c r="O10" s="22"/>
+      <c r="O10" s="20"/>
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -890,7 +967,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="21"/>
+      <c r="O11" s="19"/>
       <c r="P11" s="1"/>
     </row>
     <row r="12" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -900,7 +977,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
-      <c r="O12" s="22"/>
+      <c r="O12" s="20"/>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1959,17 +2036,17 @@
     <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="D4:E4"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -1981,7 +2058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K977"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -2001,11 +2078,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2013,11 +2090,11 @@
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -2033,19 +2110,19 @@
       <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
       <c r="H5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="10" t="s">
@@ -2057,19 +2134,19 @@
       <c r="D6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
       <c r="H6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
     </row>
     <row r="7" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="10" t="s">
@@ -2081,19 +2158,19 @@
       <c r="D7" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
       <c r="H7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="I7" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
     </row>
     <row r="8" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="13" t="s">
@@ -2105,17 +2182,17 @@
       <c r="D8" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
       <c r="H8" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="I8" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
     </row>
     <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="13" t="s">
@@ -2127,19 +2204,19 @@
       <c r="D9" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
       <c r="H9" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
     </row>
     <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="13" t="s">
@@ -2151,43 +2228,43 @@
       <c r="D10" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
       <c r="H10" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="25" t="s">
+      <c r="I10" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
     </row>
     <row r="11" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="17" t="s">
         <v>44</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="31" t="s">
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="25" t="s">
+      <c r="I11" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
     </row>
     <row r="12" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3157,12 +3234,6 @@
     <row r="977" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="I10:K10"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="E5:G5"/>
@@ -3173,6 +3244,12 @@
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="I7:K7"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="I10:K10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E10" r:id="rId1" xr:uid="{A5164392-496C-4A39-9165-C13CA7099E7B}"/>
@@ -3180,4 +3257,116 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD9EF5E1-6F8A-49D8-84FF-4C79B63CBEEA}">
+  <dimension ref="B3:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" customWidth="1"/>
+    <col min="7" max="7" width="29.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="23"/>
+      <c r="F3" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="2:7" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="B4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="63" x14ac:dyDescent="0.2">
+      <c r="B5" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="23"/>
+      <c r="C6" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrego  casos de prueba a Borrar rol
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M4.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M4.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b6b49da01230f2/Documentos/proyecto wong/Softgenix-Peru/2-Desarrollo/SCIP/pruebas-calidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="11_8BF91C39AE0E0FE7D079E26E9C7D4D10BFF76F8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31F28D13-2AE5-4571-B8B5-43F18455D871}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="11_8BF91C39AE0E0FE7D079E26E9C7D4D10BFF76F8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A42EF4D-F11A-4EB9-AD6B-6D0C82ED7FD6}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="960" windowWidth="17925" windowHeight="11460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="690" windowWidth="17925" windowHeight="11460" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CE Registrar rol" sheetId="1" r:id="rId1"/>
     <sheet name="CP Registrar rol" sheetId="2" r:id="rId2"/>
     <sheet name="CE Borrar rol" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="59">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -192,13 +193,25 @@
   </si>
   <si>
     <t>Cancelar la acción de borrado cuando se solicite</t>
+  </si>
+  <si>
+    <t>BORRAR ROL</t>
+  </si>
+  <si>
+    <t>borrado exitoso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hacer clic </t>
+  </si>
+  <si>
+    <t>eliminado correctamente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -262,6 +275,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -313,7 +333,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -336,12 +356,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -393,6 +457,21 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
@@ -400,32 +479,50 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -829,14 +926,14 @@
     <row r="4" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="22" t="s">
+      <c r="E4" s="20"/>
+      <c r="F4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="23"/>
+      <c r="G4" s="20"/>
     </row>
     <row r="5" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
@@ -860,14 +957,14 @@
       <c r="I5" s="1"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="20"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="25"/>
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="2:16" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="21" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -895,14 +992,14 @@
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="23"/>
-      <c r="C7" s="24" t="s">
+      <c r="B7" s="20"/>
+      <c r="C7" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="23" t="s">
         <v>21</v>
       </c>
       <c r="F7" s="8" t="s">
@@ -917,14 +1014,14 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="19"/>
+      <c r="O7" s="24"/>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="2:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="8" t="s">
         <v>24</v>
       </c>
@@ -937,7 +1034,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="20"/>
+      <c r="O8" s="25"/>
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -947,7 +1044,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="19"/>
+      <c r="O9" s="24"/>
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -957,7 +1054,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-      <c r="O10" s="20"/>
+      <c r="O10" s="25"/>
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -967,7 +1064,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="19"/>
+      <c r="O11" s="24"/>
       <c r="P11" s="1"/>
     </row>
     <row r="12" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -977,7 +1074,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
-      <c r="O12" s="20"/>
+      <c r="O12" s="25"/>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2036,17 +2133,17 @@
     <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="D4:E4"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -2078,11 +2175,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
     </row>
     <row r="2" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2090,11 +2187,11 @@
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -2110,19 +2207,19 @@
       <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
       <c r="H5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="10" t="s">
@@ -2134,19 +2231,19 @@
       <c r="D6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
       <c r="H6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="28" t="s">
+      <c r="I6" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
     </row>
     <row r="7" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="10" t="s">
@@ -2158,19 +2255,19 @@
       <c r="D7" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
       <c r="H7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="28" t="s">
+      <c r="I7" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
     </row>
     <row r="8" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="13" t="s">
@@ -2182,17 +2279,17 @@
       <c r="D8" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
       <c r="H8" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="28" t="s">
+      <c r="I8" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
     </row>
     <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="13" t="s">
@@ -2204,19 +2301,19 @@
       <c r="D9" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
       <c r="H9" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="28" t="s">
+      <c r="I9" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
     </row>
     <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="13" t="s">
@@ -2228,19 +2325,19 @@
       <c r="D10" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="29" t="s">
+      <c r="E10" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
       <c r="H10" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="28" t="s">
+      <c r="I10" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
     </row>
     <row r="11" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="16" t="s">
@@ -2252,19 +2349,19 @@
       <c r="D11" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
       <c r="H11" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="28" t="s">
+      <c r="I11" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
     </row>
     <row r="12" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3234,6 +3331,12 @@
     <row r="977" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="I10:K10"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="E5:G5"/>
@@ -3244,12 +3347,6 @@
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="I7:K7"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="I10:K10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E10" r:id="rId1" xr:uid="{A5164392-496C-4A39-9165-C13CA7099E7B}"/>
@@ -3263,7 +3360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD9EF5E1-6F8A-49D8-84FF-4C79B63CBEEA}">
   <dimension ref="B3:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -3278,14 +3375,14 @@
     <row r="3" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="22" t="s">
+      <c r="E3" s="20"/>
+      <c r="F3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="23"/>
+      <c r="G3" s="20"/>
     </row>
     <row r="4" spans="2:7" ht="47.25" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
@@ -3307,8 +3404,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="63" x14ac:dyDescent="0.2">
-      <c r="B5" s="24" t="s">
+    <row r="5" spans="2:7" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="B5" s="21" t="s">
         <v>48</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -3328,14 +3425,14 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="23"/>
-      <c r="C6" s="24" t="s">
+      <c r="B6" s="20"/>
+      <c r="C6" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="23" t="s">
         <v>21</v>
       </c>
       <c r="F6" s="8" t="s">
@@ -3346,10 +3443,10 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
       <c r="F7" s="8" t="s">
         <v>54</v>
       </c>
@@ -3369,4 +3466,101 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C978F1B9-0D35-4301-9395-A8E4BFF921FF}">
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+    </row>
+    <row r="6" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+    </row>
+    <row r="7" spans="1:11" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="B7" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="38"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="J7" s="41"/>
+      <c r="K7" s="42"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="I7:K7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
se actualizo casos de prueba a Borrar Rol
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M4.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M4.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b6b49da01230f2/Documentos/proyecto wong/Softgenix-Peru/2-Desarrollo/SCIP/pruebas-calidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="11_8BF91C39AE0E0FE7D079E26E9C7D4D10BFF76F8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A42EF4D-F11A-4EB9-AD6B-6D0C82ED7FD6}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="11_8BF91C39AE0E0FE7D079E26E9C7D4D10BFF76F8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4999FB52-ABED-470F-84BA-C4EEC9719AB8}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="690" windowWidth="17925" windowHeight="11460" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7320" yWindow="3630" windowWidth="17925" windowHeight="11460" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CE Registrar rol" sheetId="1" r:id="rId1"/>
     <sheet name="CP Registrar rol" sheetId="2" r:id="rId2"/>
     <sheet name="CE Borrar rol" sheetId="3" r:id="rId3"/>
-    <sheet name="Hoja1" sheetId="4" r:id="rId4"/>
+    <sheet name="CP Borrar rol" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="62">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -205,6 +205,15 @@
   </si>
   <si>
     <t>eliminado correctamente</t>
+  </si>
+  <si>
+    <t>borrado fallido</t>
+  </si>
+  <si>
+    <t>no se elimina</t>
+  </si>
+  <si>
+    <t>Rol no se elimina</t>
   </si>
 </sst>
 </file>
@@ -405,7 +414,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -457,20 +466,14 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -479,32 +482,38 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -521,6 +530,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -926,14 +944,14 @@
     <row r="4" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="19" t="s">
+      <c r="E4" s="26"/>
+      <c r="F4" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="20"/>
+      <c r="G4" s="26"/>
     </row>
     <row r="5" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
@@ -957,14 +975,14 @@
       <c r="I5" s="1"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="25"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="23"/>
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="2:16" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="27" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -992,14 +1010,14 @@
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="20"/>
-      <c r="C7" s="21" t="s">
+      <c r="B7" s="26"/>
+      <c r="C7" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="29" t="s">
         <v>21</v>
       </c>
       <c r="F7" s="8" t="s">
@@ -1014,14 +1032,14 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="24"/>
+      <c r="O7" s="22"/>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="2:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
       <c r="F8" s="8" t="s">
         <v>24</v>
       </c>
@@ -1034,7 +1052,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="25"/>
+      <c r="O8" s="23"/>
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1044,7 +1062,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="24"/>
+      <c r="O9" s="22"/>
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1054,7 +1072,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-      <c r="O10" s="25"/>
+      <c r="O10" s="23"/>
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1064,7 +1082,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="24"/>
+      <c r="O11" s="22"/>
       <c r="P11" s="1"/>
     </row>
     <row r="12" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1074,7 +1092,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
-      <c r="O12" s="25"/>
+      <c r="O12" s="23"/>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2133,17 +2151,17 @@
     <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="D4:E4"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -2175,11 +2193,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
     </row>
     <row r="2" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2187,11 +2205,11 @@
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -2207,19 +2225,19 @@
       <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
       <c r="H5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="10" t="s">
@@ -2231,19 +2249,19 @@
       <c r="D6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
       <c r="H6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="29" t="s">
+      <c r="I6" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
     </row>
     <row r="7" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="10" t="s">
@@ -2255,19 +2273,19 @@
       <c r="D7" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
       <c r="H7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="29" t="s">
+      <c r="I7" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
     </row>
     <row r="8" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="13" t="s">
@@ -2279,17 +2297,17 @@
       <c r="D8" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
       <c r="H8" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="29" t="s">
+      <c r="I8" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
     </row>
     <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="13" t="s">
@@ -2301,19 +2319,19 @@
       <c r="D9" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
       <c r="H9" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="29" t="s">
+      <c r="I9" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
     </row>
     <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="13" t="s">
@@ -2325,19 +2343,19 @@
       <c r="D10" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
       <c r="H10" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="29" t="s">
+      <c r="I10" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
     </row>
     <row r="11" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="16" t="s">
@@ -2349,19 +2367,19 @@
       <c r="D11" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
       <c r="H11" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="29" t="s">
+      <c r="I11" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
     </row>
     <row r="12" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3331,12 +3349,6 @@
     <row r="977" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="I10:K10"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="E5:G5"/>
@@ -3347,6 +3359,12 @@
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="I7:K7"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="I10:K10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E10" r:id="rId1" xr:uid="{A5164392-496C-4A39-9165-C13CA7099E7B}"/>
@@ -3375,14 +3393,14 @@
     <row r="3" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="19" t="s">
+      <c r="E3" s="26"/>
+      <c r="F3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="20"/>
+      <c r="G3" s="26"/>
     </row>
     <row r="4" spans="2:7" ht="47.25" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
@@ -3405,7 +3423,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="27" t="s">
         <v>48</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -3425,14 +3443,14 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="20"/>
-      <c r="C6" s="21" t="s">
+      <c r="B6" s="26"/>
+      <c r="C6" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="29" t="s">
         <v>21</v>
       </c>
       <c r="F6" s="8" t="s">
@@ -3443,10 +3461,10 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
       <c r="F7" s="8" t="s">
         <v>54</v>
       </c>
@@ -3470,10 +3488,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C978F1B9-0D35-4301-9395-A8E4BFF921FF}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3484,27 +3502,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
     </row>
-    <row r="6" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
@@ -3514,28 +3532,28 @@
       <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
       <c r="H6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-    </row>
-    <row r="7" spans="1:11" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="B7" s="34" t="s">
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+    </row>
+    <row r="7" spans="1:11" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="B7" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="21" t="s">
         <v>29</v>
       </c>
       <c r="E7" s="37" t="s">
@@ -3543,7 +3561,7 @@
       </c>
       <c r="F7" s="38"/>
       <c r="G7" s="39"/>
-      <c r="H7" s="35" t="s">
+      <c r="H7" s="20" t="s">
         <v>58</v>
       </c>
       <c r="I7" s="40" t="s">
@@ -3552,8 +3570,86 @@
       <c r="J7" s="41"/>
       <c r="K7" s="42"/>
     </row>
+    <row r="8" spans="1:11" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="B8" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+    </row>
+    <row r="9" spans="1:11" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="B9" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" s="45"/>
+      <c r="K9" s="45"/>
+    </row>
+    <row r="10" spans="1:11" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="B10" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" s="45"/>
+      <c r="K10" s="45"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="12">
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="I10:K10"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="E6:G6"/>

</xml_diff>

<commit_message>
Se agrego la tabla de resultados al modulo funcional Rol
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M4.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M4.xlsx
@@ -8,18 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b6b49da01230f2/Documentos/proyecto wong/Softgenix-Peru/2-Desarrollo/SCIP/pruebas-calidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="11_8BF91C39AE0E0FE7D079E26E9C7D4D10BFF76F8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4999FB52-ABED-470F-84BA-C4EEC9719AB8}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="11_8BF91C39AE0E0FE7D079E26E9C7D4D10BFF76F8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{305AA029-2D07-49F6-BB41-3FDC75B84827}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="3630" windowWidth="17925" windowHeight="11460" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7320" yWindow="3630" windowWidth="17925" windowHeight="11460" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CE Registrar rol" sheetId="1" r:id="rId1"/>
     <sheet name="CP Registrar rol" sheetId="2" r:id="rId2"/>
     <sheet name="CE Borrar rol" sheetId="3" r:id="rId3"/>
     <sheet name="CP Borrar rol" sheetId="4" r:id="rId4"/>
+    <sheet name="Tabla de resultados" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="oCOje7eQ+BNatKuPs7RwyjtQZmaEt8Ox0GG8W65hv9c="/>
     </ext>
@@ -28,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="72">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -214,13 +226,43 @@
   </si>
   <si>
     <t>Rol no se elimina</t>
+  </si>
+  <si>
+    <t>Funcionalidad</t>
+  </si>
+  <si>
+    <t>Casos de pruebas no válidadas</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Porcentaje con defectos</t>
+  </si>
+  <si>
+    <t>Porcentaje sin defectos</t>
+  </si>
+  <si>
+    <t>Con Defectos</t>
+  </si>
+  <si>
+    <t>Sin Defectos</t>
+  </si>
+  <si>
+    <t>Registrar Rol</t>
+  </si>
+  <si>
+    <t>Eliminar rol</t>
+  </si>
+  <si>
+    <t>Caso de pruebas validadas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -291,8 +333,15 @@
       <name val="Garamond"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -339,6 +388,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4A7D6"/>
         <bgColor rgb="FFB4A7D6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -410,11 +465,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -475,6 +531,27 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
@@ -482,32 +559,20 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -532,19 +597,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -717,10 +789,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -944,14 +1012,14 @@
     <row r="4" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="26"/>
-      <c r="F4" s="25" t="s">
+      <c r="E4" s="25"/>
+      <c r="F4" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="26"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
@@ -975,14 +1043,14 @@
       <c r="I5" s="1"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="24"/>
-      <c r="O5" s="23"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="30"/>
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="2:16" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="26" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -1010,14 +1078,14 @@
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="26"/>
-      <c r="C7" s="27" t="s">
+      <c r="B7" s="25"/>
+      <c r="C7" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="28" t="s">
         <v>21</v>
       </c>
       <c r="F7" s="8" t="s">
@@ -1032,14 +1100,14 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="22"/>
+      <c r="O7" s="29"/>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="2:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
       <c r="F8" s="8" t="s">
         <v>24</v>
       </c>
@@ -1052,7 +1120,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="23"/>
+      <c r="O8" s="30"/>
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1062,7 +1130,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="22"/>
+      <c r="O9" s="29"/>
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1072,7 +1140,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-      <c r="O10" s="23"/>
+      <c r="O10" s="30"/>
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1082,7 +1150,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="22"/>
+      <c r="O11" s="29"/>
       <c r="P11" s="1"/>
     </row>
     <row r="12" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1092,7 +1160,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
-      <c r="O12" s="23"/>
+      <c r="O12" s="30"/>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2151,17 +2219,17 @@
     <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="D4:E4"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -2193,11 +2261,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
     </row>
     <row r="2" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2205,11 +2273,11 @@
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -2225,19 +2293,19 @@
       <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
       <c r="H5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="I5" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="10" t="s">
@@ -2249,19 +2317,19 @@
       <c r="D6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
       <c r="H6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
     </row>
     <row r="7" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="10" t="s">
@@ -2273,19 +2341,19 @@
       <c r="D7" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
       <c r="H7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="31" t="s">
+      <c r="I7" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
     </row>
     <row r="8" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="13" t="s">
@@ -2297,17 +2365,17 @@
       <c r="D8" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
       <c r="H8" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="31" t="s">
+      <c r="I8" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
     </row>
     <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="13" t="s">
@@ -2319,19 +2387,19 @@
       <c r="D9" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
       <c r="H9" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="31" t="s">
+      <c r="I9" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
     </row>
     <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="13" t="s">
@@ -2343,19 +2411,19 @@
       <c r="D10" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
       <c r="H10" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="31" t="s">
+      <c r="I10" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
     </row>
     <row r="11" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="16" t="s">
@@ -2367,19 +2435,19 @@
       <c r="D11" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
       <c r="H11" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="31" t="s">
+      <c r="I11" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
     </row>
     <row r="12" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3349,6 +3417,12 @@
     <row r="977" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="I10:K10"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="E5:G5"/>
@@ -3359,12 +3433,6 @@
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="I7:K7"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="I10:K10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E10" r:id="rId1" xr:uid="{A5164392-496C-4A39-9165-C13CA7099E7B}"/>
@@ -3393,14 +3461,14 @@
     <row r="3" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="25" t="s">
+      <c r="E3" s="25"/>
+      <c r="F3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="26"/>
+      <c r="G3" s="25"/>
     </row>
     <row r="4" spans="2:7" ht="47.25" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
@@ -3423,7 +3491,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>48</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -3443,14 +3511,14 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="26"/>
-      <c r="C6" s="27" t="s">
+      <c r="B6" s="25"/>
+      <c r="C6" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="28" t="s">
         <v>21</v>
       </c>
       <c r="F6" s="8" t="s">
@@ -3461,10 +3529,10 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
       <c r="F7" s="8" t="s">
         <v>54</v>
       </c>
@@ -3490,7 +3558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C978F1B9-0D35-4301-9395-A8E4BFF921FF}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -3502,21 +3570,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
@@ -3532,19 +3600,19 @@
       <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
       <c r="H6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
     </row>
     <row r="7" spans="1:11" ht="31.5" x14ac:dyDescent="0.2">
       <c r="B7" s="19" t="s">
@@ -3556,106 +3624,233 @@
       <c r="D7" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="E7" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="38"/>
-      <c r="G7" s="39"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="42"/>
       <c r="H7" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="I7" s="40" t="s">
+      <c r="I7" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="J7" s="41"/>
-      <c r="K7" s="42"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="45"/>
     </row>
     <row r="8" spans="1:11" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
       <c r="H8" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="I8" s="45" t="s">
+      <c r="I8" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
     </row>
     <row r="9" spans="1:11" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="22" t="s">
         <v>34</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
       <c r="H9" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="45" t="s">
+      <c r="I9" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="J9" s="45"/>
-      <c r="K9" s="45"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
     </row>
     <row r="10" spans="1:11" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="22" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="44" t="s">
+      <c r="D10" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
       <c r="H10" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="45" t="s">
+      <c r="I10" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="J10" s="45"/>
-      <c r="K10" s="45"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="I7:K7"/>
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="I10:K10"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="I7:K7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F864E1-46A0-4B54-9229-B3DCC9AF700C}">
+  <dimension ref="B3:H7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B3" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="46" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+    </row>
+    <row r="5" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B5" s="46"/>
+      <c r="C5" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+    </row>
+    <row r="6" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="49">
+        <v>3</v>
+      </c>
+      <c r="D6" s="49">
+        <v>2</v>
+      </c>
+      <c r="E6" s="49">
+        <v>1</v>
+      </c>
+      <c r="F6" s="49">
+        <f>SUM(C6:E6)</f>
+        <v>6</v>
+      </c>
+      <c r="G6" s="50">
+        <f>C6/F6</f>
+        <v>0.5</v>
+      </c>
+      <c r="H6" s="50">
+        <f>D6/F6</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="49">
+        <v>0</v>
+      </c>
+      <c r="D7" s="49">
+        <v>4</v>
+      </c>
+      <c r="E7" s="49">
+        <v>0</v>
+      </c>
+      <c r="F7" s="49">
+        <f>SUM(C7:E7)</f>
+        <v>4</v>
+      </c>
+      <c r="G7" s="50">
+        <f t="shared" ref="G7" si="0">C7/F7</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="50">
+        <f t="shared" ref="H7" si="1">D7/F7</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:D4"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="H3:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se actualizo la tabla de resultados al modulo funcional Rol
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M4.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b6b49da01230f2/Documentos/proyecto wong/Softgenix-Peru/2-Desarrollo/SCIP/pruebas-calidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="11_8BF91C39AE0E0FE7D079E26E9C7D4D10BFF76F8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{305AA029-2D07-49F6-BB41-3FDC75B84827}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="11_8BF91C39AE0E0FE7D079E26E9C7D4D10BFF76F8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DA3F225-5251-405A-9911-134EA5698C70}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="3630" windowWidth="17925" windowHeight="11460" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CE Registrar rol" sheetId="1" r:id="rId1"/>
@@ -537,6 +537,25 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -552,27 +571,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -597,20 +606,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -629,6 +629,877 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Tabla de resultados'!$G$3:$G$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Porcentaje con defectos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Tabla de resultados'!$B$6:$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Registrar Rol</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Eliminar rol</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Tabla de resultados'!$G$6:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-359D-45B6-AAF8-EFD7E2BB067F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Tabla de resultados'!$H$3:$H$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Porcentaje sin defectos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Tabla de resultados'!$H$6:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-359D-45B6-AAF8-EFD7E2BB067F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1456856639"/>
+        <c:axId val="1456853759"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1456856639"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1456853759"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1456853759"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1456856639"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-PE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-PE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -789,6 +1660,51 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>904875</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0262B427-54A6-628E-5D67-2E72A1A6BDDF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1012,14 +1928,14 @@
     <row r="4" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="24" t="s">
+      <c r="E4" s="32"/>
+      <c r="F4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="25"/>
+      <c r="G4" s="32"/>
     </row>
     <row r="5" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
@@ -1043,14 +1959,14 @@
       <c r="I5" s="1"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="29"/>
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="2:16" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="33" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -1078,14 +1994,14 @@
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="25"/>
-      <c r="C7" s="26" t="s">
+      <c r="B7" s="32"/>
+      <c r="C7" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="35" t="s">
         <v>21</v>
       </c>
       <c r="F7" s="8" t="s">
@@ -1100,14 +2016,14 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="29"/>
+      <c r="O7" s="28"/>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="2:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
       <c r="F8" s="8" t="s">
         <v>24</v>
       </c>
@@ -1120,7 +2036,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="30"/>
+      <c r="O8" s="29"/>
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1130,7 +2046,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="29"/>
+      <c r="O9" s="28"/>
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1140,7 +2056,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-      <c r="O10" s="30"/>
+      <c r="O10" s="29"/>
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1150,7 +2066,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="29"/>
+      <c r="O11" s="28"/>
       <c r="P11" s="1"/>
     </row>
     <row r="12" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1160,7 +2076,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
-      <c r="O12" s="30"/>
+      <c r="O12" s="29"/>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2219,17 +3135,17 @@
     <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="D4:E4"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -2261,11 +3177,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2273,11 +3189,11 @@
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -2293,19 +3209,19 @@
       <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
       <c r="H5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="I5" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="10" t="s">
@@ -2317,19 +3233,19 @@
       <c r="D6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
       <c r="H6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="34" t="s">
+      <c r="I6" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
     </row>
     <row r="7" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="10" t="s">
@@ -2341,19 +3257,19 @@
       <c r="D7" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
       <c r="H7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="34" t="s">
+      <c r="I7" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
     </row>
     <row r="8" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="13" t="s">
@@ -2365,17 +3281,17 @@
       <c r="D8" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
       <c r="H8" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="34" t="s">
+      <c r="I8" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
     </row>
     <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="13" t="s">
@@ -2387,19 +3303,19 @@
       <c r="D9" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
       <c r="H9" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="34" t="s">
+      <c r="I9" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
     </row>
     <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="13" t="s">
@@ -2411,19 +3327,19 @@
       <c r="D10" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="36" t="s">
+      <c r="E10" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
       <c r="H10" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="34" t="s">
+      <c r="I10" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
     </row>
     <row r="11" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="16" t="s">
@@ -2435,19 +3351,19 @@
       <c r="D11" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="33" t="s">
+      <c r="E11" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
       <c r="H11" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="34" t="s">
+      <c r="I11" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
     </row>
     <row r="12" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3417,12 +4333,6 @@
     <row r="977" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="I10:K10"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="E5:G5"/>
@@ -3433,6 +4343,12 @@
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="I7:K7"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="I10:K10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E10" r:id="rId1" xr:uid="{A5164392-496C-4A39-9165-C13CA7099E7B}"/>
@@ -3461,14 +4377,14 @@
     <row r="3" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="24" t="s">
+      <c r="E3" s="32"/>
+      <c r="F3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="25"/>
+      <c r="G3" s="32"/>
     </row>
     <row r="4" spans="2:7" ht="47.25" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
@@ -3491,7 +4407,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="33" t="s">
         <v>48</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -3511,14 +4427,14 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="25"/>
-      <c r="C6" s="26" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="35" t="s">
         <v>21</v>
       </c>
       <c r="F6" s="8" t="s">
@@ -3529,10 +4445,10 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
       <c r="F7" s="8" t="s">
         <v>54</v>
       </c>
@@ -3570,21 +4486,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
@@ -3600,19 +4516,19 @@
       <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
       <c r="H6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="24" t="s">
+      <c r="I6" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
     </row>
     <row r="7" spans="1:11" ht="31.5" x14ac:dyDescent="0.2">
       <c r="B7" s="19" t="s">
@@ -3624,19 +4540,19 @@
       <c r="D7" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="41"/>
-      <c r="G7" s="42"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="45"/>
       <c r="H7" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="I7" s="43" t="s">
+      <c r="I7" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="J7" s="44"/>
-      <c r="K7" s="45"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="48"/>
     </row>
     <row r="8" spans="1:11" ht="31.5" x14ac:dyDescent="0.2">
       <c r="B8" s="22" t="s">
@@ -3648,19 +4564,19 @@
       <c r="D8" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
       <c r="H8" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="I8" s="37" t="s">
+      <c r="I8" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
     </row>
     <row r="9" spans="1:11" ht="31.5" x14ac:dyDescent="0.2">
       <c r="B9" s="22" t="s">
@@ -3672,19 +4588,19 @@
       <c r="D9" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
       <c r="H9" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="37" t="s">
+      <c r="I9" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
     </row>
     <row r="10" spans="1:11" ht="31.5" x14ac:dyDescent="0.2">
       <c r="B10" s="22" t="s">
@@ -3696,34 +4612,34 @@
       <c r="D10" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="E10" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
       <c r="H10" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="37" t="s">
+      <c r="I10" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="I10:K10"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="I7:K7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="I10:K10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3734,7 +4650,7 @@
   <dimension ref="B3:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3749,109 +4665,110 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46" t="s">
+      <c r="D3" s="50"/>
+      <c r="E3" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="H3" s="50" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
     </row>
-    <row r="5" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="46"/>
-      <c r="C5" s="47" t="s">
+    <row r="5" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="50"/>
+      <c r="C5" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
     </row>
-    <row r="6" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="48" t="s">
+    <row r="6" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="49">
+      <c r="C6" s="26">
         <v>3</v>
       </c>
-      <c r="D6" s="49">
+      <c r="D6" s="26">
         <v>2</v>
       </c>
-      <c r="E6" s="49">
+      <c r="E6" s="26">
         <v>1</v>
       </c>
-      <c r="F6" s="49">
+      <c r="F6" s="26">
         <f>SUM(C6:E6)</f>
         <v>6</v>
       </c>
-      <c r="G6" s="50">
+      <c r="G6" s="27">
         <f>C6/F6</f>
         <v>0.5</v>
       </c>
-      <c r="H6" s="50">
+      <c r="H6" s="27">
         <f>D6/F6</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="48" t="s">
+    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="49">
+      <c r="C7" s="26">
         <v>0</v>
       </c>
-      <c r="D7" s="49">
+      <c r="D7" s="26">
         <v>4</v>
       </c>
-      <c r="E7" s="49">
+      <c r="E7" s="26">
         <v>0</v>
       </c>
-      <c r="F7" s="49">
+      <c r="F7" s="26">
         <f>SUM(C7:E7)</f>
         <v>4</v>
       </c>
-      <c r="G7" s="50">
+      <c r="G7" s="27">
         <f t="shared" ref="G7" si="0">C7/F7</f>
         <v>0</v>
       </c>
-      <c r="H7" s="50">
+      <c r="H7" s="27">
         <f t="shared" ref="H7" si="1">D7/F7</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="H3:H5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:D4"/>
     <mergeCell ref="E3:E5"/>
     <mergeCell ref="F3:F5"/>
     <mergeCell ref="G3:G5"/>
-    <mergeCell ref="H3:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>